<commit_message>
Brief agenda en planning aangepast
</commit_message>
<xml_diff>
--- a/Agenda en notulen/Agenda's/Agenda_Week_1.xlsx
+++ b/Agenda en notulen/Agenda's/Agenda_Week_1.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Project_P5\Agenda en notulen\Agenda's\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="19440" windowHeight="12210"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -21,7 +26,7 @@
     <author>Fer</author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="0">
+    <comment ref="H18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -199,17 +204,17 @@
     <t>Peilingslijst</t>
   </si>
   <si>
-    <t>Tijd: 15:00</t>
+    <t>Tijd: 10:20 t/m 10:20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -616,7 +621,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -658,7 +663,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -690,9 +695,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -724,6 +730,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -899,17 +906,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -924,8 +931,8 @@
     <col min="16" max="16" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="52"/>
       <c r="C2" s="53"/>
       <c r="D2" s="53"/>
@@ -935,7 +942,7 @@
       <c r="H2" s="54"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="55" t="s">
         <v>20</v>
       </c>
@@ -949,7 +956,7 @@
       <c r="H3" s="60"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="67" t="s">
         <v>33</v>
       </c>
@@ -961,7 +968,7 @@
       <c r="H4" s="63"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="2:10" ht="15.75" thickBot="1">
+    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="70" t="s">
         <v>26</v>
       </c>
@@ -973,7 +980,7 @@
       <c r="H5" s="66"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="2:10" ht="15.75" thickBot="1">
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -991,7 +998,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="2:10" ht="18">
+    <row r="7" spans="2:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="C7" s="13"/>
       <c r="D7" s="14"/>
@@ -1001,7 +1008,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>17</v>
       </c>
@@ -1022,7 +1029,7 @@
       <c r="I8" s="19"/>
       <c r="J8" s="20"/>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>25</v>
       </c>
@@ -1041,7 +1048,7 @@
       <c r="H9" s="18"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
@@ -1061,7 +1068,7 @@
       <c r="H10" s="18"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
         <v>18</v>
       </c>
@@ -1081,7 +1088,7 @@
       <c r="H11" s="25"/>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
         <v>18</v>
       </c>
@@ -1101,7 +1108,7 @@
       <c r="H12" s="25"/>
       <c r="I12" s="19"/>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>18</v>
       </c>
@@ -1121,7 +1128,7 @@
       <c r="H13" s="25"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="22"/>
@@ -1130,7 +1137,7 @@
       <c r="H14" s="18"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="22"/>
       <c r="C15" s="13"/>
       <c r="D15" s="22"/>
@@ -1139,7 +1146,7 @@
       <c r="H15" s="18"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="2:10" ht="15.75" thickBot="1">
+    <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
       <c r="D16" s="27"/>
@@ -1148,7 +1155,7 @@
       <c r="G16" s="30"/>
       <c r="H16" s="31"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="32"/>
       <c r="C17" s="33">
         <f>SUM(C8:C16)</f>
@@ -1166,7 +1173,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" s="37"/>
       <c r="C18" s="33"/>
       <c r="D18" s="38" t="s">
@@ -1181,7 +1188,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" s="37"/>
       <c r="C19" s="33"/>
       <c r="D19" s="38" t="s">
@@ -1194,7 +1201,7 @@
       <c r="G19" s="39"/>
       <c r="H19" s="40"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" s="37"/>
       <c r="C20" s="33"/>
       <c r="D20" s="38" t="s">
@@ -1207,7 +1214,7 @@
       <c r="G20" s="39"/>
       <c r="H20" s="40"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1">
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="41"/>
       <c r="C21" s="42"/>
       <c r="D21" s="43" t="s">
@@ -1220,12 +1227,12 @@
       <c r="G21" s="45"/>
       <c r="H21" s="46"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E23" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" s="47"/>
       <c r="E24" s="4">
         <v>1</v>
@@ -1233,7 +1240,7 @@
       <c r="F24" s="48"/>
       <c r="I24" s="49"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="E25" s="4">
         <v>2</v>
@@ -1241,7 +1248,7 @@
       <c r="F25" s="21"/>
       <c r="I25" s="49"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="E26" s="4">
         <v>3</v>
@@ -1249,7 +1256,7 @@
       <c r="F26" s="23"/>
       <c r="I26" s="49"/>
     </row>
-    <row r="27" spans="1:9" s="1" customFormat="1">
+    <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="D27" s="3"/>
       <c r="E27" s="4">
@@ -1260,14 +1267,14 @@
       <c r="H27" s="50"/>
       <c r="I27" s="51"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="E28" s="4">
         <v>5</v>
       </c>
       <c r="I28" s="49"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="E29" s="4">
         <v>6</v>
@@ -1275,7 +1282,7 @@
       <c r="F29" s="48"/>
       <c r="I29" s="49"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="E30" s="4">
         <v>7</v>
@@ -1283,18 +1290,18 @@
       <c r="F30" s="48"/>
       <c r="I30" s="49"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="F31" s="48"/>
       <c r="I31" s="49"/>
     </row>
-    <row r="32" spans="1:9" ht="14.25" customHeight="1">
+    <row r="32" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E32" s="4" t="s">
         <v>16</v>
       </c>
       <c r="I32" s="49"/>
     </row>
-    <row r="33" spans="5:12" ht="14.25" customHeight="1">
+    <row r="33" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E33" s="4">
         <v>1</v>
       </c>
@@ -1306,7 +1313,7 @@
       <c r="K33" s="21"/>
       <c r="L33" s="21"/>
     </row>
-    <row r="34" spans="5:12" ht="14.25" customHeight="1">
+    <row r="34" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="4">
         <v>2</v>
       </c>
@@ -1318,7 +1325,7 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
     </row>
-    <row r="35" spans="5:12" ht="14.25" customHeight="1">
+    <row r="35" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="4">
         <v>3</v>
       </c>
@@ -1330,76 +1337,76 @@
       <c r="K35" s="21"/>
       <c r="L35" s="21"/>
     </row>
-    <row r="36" spans="5:12" ht="14.25" customHeight="1">
+    <row r="36" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="5:12" ht="10.5" customHeight="1">
+    <row r="37" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I37" s="5"/>
     </row>
-    <row r="38" spans="5:12" ht="10.5" customHeight="1">
+    <row r="38" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I38" s="5"/>
     </row>
-    <row r="39" spans="5:12" ht="10.5" customHeight="1">
+    <row r="39" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="5:12" ht="10.5" customHeight="1">
+    <row r="40" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="5:12" ht="10.5" customHeight="1">
+    <row r="41" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="5:12">
+    <row r="42" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="5:12">
+    <row r="43" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="5:12">
+    <row r="44" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="5:12">
+    <row r="45" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="5:12">
+    <row r="46" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="5:12">
+    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I47" s="5"/>
     </row>
-    <row r="48" spans="5:12">
+    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I48" s="5"/>
     </row>
-    <row r="49" spans="9:9">
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I49" s="5"/>
     </row>
-    <row r="50" spans="9:9">
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I50" s="5"/>
     </row>
-    <row r="51" spans="9:9">
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I51" s="5"/>
     </row>
-    <row r="52" spans="9:9">
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I52" s="5"/>
     </row>
-    <row r="53" spans="9:9">
+    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I53" s="5"/>
     </row>
-    <row r="54" spans="9:9">
+    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I54" s="5"/>
     </row>
-    <row r="55" spans="9:9">
+    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I55" s="5"/>
     </row>
-    <row r="56" spans="9:9">
+    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I56" s="5"/>
     </row>
-    <row r="57" spans="9:9">
+    <row r="57" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I57" s="5"/>
     </row>
-    <row r="58" spans="9:9">
+    <row r="58" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I58" s="5"/>
     </row>
-    <row r="59" spans="9:9">
+    <row r="59" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I59" s="5"/>
     </row>
   </sheetData>
@@ -1417,45 +1424,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C8428B090D81B34DA19517DD6F855647" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="461551752daf7baccd316804784cc5e1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b118b0825d757084c8d1e1ffd33f200c">
     <xsd:element name="properties">
@@ -1504,10 +1496,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8B5FF3C-AF10-4D69-A171-7686A3EF9E92}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1521,16 +1535,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8B5FF3C-AF10-4D69-A171-7686A3EF9E92}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Agenda Changed, Plan van aanpak changed
</commit_message>
<xml_diff>
--- a/Agenda en notulen/Agenda's/Agenda_Week_1.xlsx
+++ b/Agenda en notulen/Agenda's/Agenda_Week_1.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Project_P5\Agenda en notulen\Agenda's\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="19440" windowHeight="12210"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -26,7 +21,7 @@
     <author>Fer</author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="0" shapeId="0">
+    <comment ref="H18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>wie</t>
   </si>
@@ -162,9 +157,6 @@
     <t>Groep</t>
   </si>
   <si>
-    <t xml:space="preserve">Notulen aan :Alle betrokkenen </t>
-  </si>
-  <si>
     <t>Locatie: Lokaal BN0330</t>
   </si>
   <si>
@@ -174,18 +166,6 @@
     <t>Vaststellen volgende vergadering</t>
   </si>
   <si>
-    <t xml:space="preserve"> AGENDA Bespreking voortgang Projectgroep 6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agenda aan :Alle betrokkenen </t>
-  </si>
-  <si>
-    <t>Kevin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datum:15-09-2014 </t>
-  </si>
-  <si>
     <t>Plan van aanpak</t>
   </si>
   <si>
@@ -195,26 +175,44 @@
     <t>Communicatie bij afwezigheid</t>
   </si>
   <si>
-    <t>Plan van aanpak bespreken</t>
-  </si>
-  <si>
     <t>MS-project bestand</t>
   </si>
   <si>
     <t>Peilingslijst</t>
   </si>
   <si>
-    <t>Tijd: 10:20 t/m 10:20</t>
+    <t xml:space="preserve"> AGENDA Project: Barroc-IT voortgangsvergadering van Projectgroep 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agenda aan :P. Hoek, K. Ly, M. Havermans, F.van Krimpen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notulen aan :F. van Krimpen, Github, P. Hoek </t>
+  </si>
+  <si>
+    <t>Plan van aanpak bespreken voor inlevering</t>
+  </si>
+  <si>
+    <t>Tijd: 10:00 t/m 10:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datum:18-09-2014 </t>
+  </si>
+  <si>
+    <t>Mededelingen</t>
+  </si>
+  <si>
+    <t>Goed teamsverband</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,7 +619,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -663,7 +661,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -695,10 +693,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -730,7 +727,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -906,17 +902,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -931,8 +927,8 @@
     <col min="16" max="16" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1">
       <c r="B2" s="52"/>
       <c r="C2" s="53"/>
       <c r="D2" s="53"/>
@@ -942,23 +938,23 @@
       <c r="H2" s="54"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10">
       <c r="B3" s="55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="56"/>
       <c r="D3" s="57"/>
       <c r="E3" s="58" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F3" s="59"/>
       <c r="G3" s="59"/>
       <c r="H3" s="60"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="B4" s="67" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="69"/>
@@ -968,9 +964,9 @@
       <c r="H4" s="63"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="15.75" thickBot="1">
       <c r="B5" s="70" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C5" s="71"/>
       <c r="D5" s="72"/>
@@ -980,7 +976,7 @@
       <c r="H5" s="66"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="15.75" thickBot="1">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -998,7 +994,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="2:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="18">
       <c r="B7" s="12"/>
       <c r="C7" s="13"/>
       <c r="D7" s="14"/>
@@ -1008,12 +1004,12 @@
       <c r="H7" s="18"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="B8" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>12</v>
@@ -1022,19 +1018,19 @@
         <v>1</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="18"/>
       <c r="I8" s="19"/>
       <c r="J8" s="20"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="B9" s="13" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C9" s="13">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>5</v>
@@ -1042,18 +1038,18 @@
       <c r="E9" s="15">
         <v>2</v>
       </c>
-      <c r="F9" s="21" t="s">
-        <v>29</v>
+      <c r="F9" t="s">
+        <v>33</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="B10" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="13">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>5</v>
@@ -1062,18 +1058,18 @@
         <v>3</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="B11" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="13">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>7</v>
@@ -1081,14 +1077,14 @@
       <c r="E11" s="15">
         <v>4</v>
       </c>
-      <c r="F11" s="23" t="s">
-        <v>30</v>
+      <c r="F11" s="21" t="s">
+        <v>23</v>
       </c>
       <c r="G11" s="24"/>
       <c r="H11" s="25"/>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10">
       <c r="B12" s="13" t="s">
         <v>18</v>
       </c>
@@ -1101,19 +1097,19 @@
       <c r="E12" s="15">
         <v>5</v>
       </c>
-      <c r="F12" s="21" t="s">
-        <v>22</v>
+      <c r="F12" s="23" t="s">
+        <v>30</v>
       </c>
       <c r="G12" s="24"/>
       <c r="H12" s="25"/>
       <c r="I12" s="19"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10">
       <c r="B13" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>5</v>
@@ -1121,23 +1117,34 @@
       <c r="E13" s="15">
         <v>6</v>
       </c>
-      <c r="F13" s="26" t="s">
-        <v>8</v>
+      <c r="F13" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="G13" s="24"/>
       <c r="H13" s="25"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="15"/>
+    <row r="14" spans="2:10">
+      <c r="B14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="13">
+        <v>5</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="15">
+        <v>7</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="G14" s="17"/>
       <c r="H14" s="18"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10">
       <c r="B15" s="22"/>
       <c r="C15" s="13"/>
       <c r="D15" s="22"/>
@@ -1146,7 +1153,7 @@
       <c r="H15" s="18"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="15.75" thickBot="1">
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
       <c r="D16" s="27"/>
@@ -1155,11 +1162,11 @@
       <c r="G16" s="30"/>
       <c r="H16" s="31"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="B17" s="32"/>
       <c r="C17" s="33">
         <f>SUM(C8:C16)</f>
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D17" s="33" t="s">
         <v>6</v>
@@ -1170,10 +1177,10 @@
       <c r="F17" s="35"/>
       <c r="G17" s="35"/>
       <c r="H17" s="36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="B18" s="37"/>
       <c r="C18" s="33"/>
       <c r="D18" s="38" t="s">
@@ -1185,10 +1192,10 @@
       <c r="F18" s="39"/>
       <c r="G18" s="39"/>
       <c r="H18" s="36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="B19" s="37"/>
       <c r="C19" s="33"/>
       <c r="D19" s="38" t="s">
@@ -1201,7 +1208,7 @@
       <c r="G19" s="39"/>
       <c r="H19" s="40"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="B20" s="37"/>
       <c r="C20" s="33"/>
       <c r="D20" s="38" t="s">
@@ -1214,7 +1221,7 @@
       <c r="G20" s="39"/>
       <c r="H20" s="40"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15.75" thickBot="1">
       <c r="B21" s="41"/>
       <c r="C21" s="42"/>
       <c r="D21" s="43" t="s">
@@ -1227,20 +1234,22 @@
       <c r="G21" s="45"/>
       <c r="H21" s="46"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="E23" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="B24" s="47"/>
       <c r="E24" s="4">
         <v>1</v>
       </c>
-      <c r="F24" s="48"/>
+      <c r="F24" s="48" t="s">
+        <v>34</v>
+      </c>
       <c r="I24" s="49"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="C25" s="1"/>
       <c r="E25" s="4">
         <v>2</v>
@@ -1248,7 +1257,7 @@
       <c r="F25" s="21"/>
       <c r="I25" s="49"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="C26" s="1"/>
       <c r="E26" s="4">
         <v>3</v>
@@ -1256,7 +1265,7 @@
       <c r="F26" s="23"/>
       <c r="I26" s="49"/>
     </row>
-    <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="1" customFormat="1">
       <c r="A27"/>
       <c r="D27" s="3"/>
       <c r="E27" s="4">
@@ -1267,14 +1276,14 @@
       <c r="H27" s="50"/>
       <c r="I27" s="51"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="1"/>
       <c r="E28" s="4">
         <v>5</v>
       </c>
       <c r="I28" s="49"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="1"/>
       <c r="E29" s="4">
         <v>6</v>
@@ -1282,7 +1291,7 @@
       <c r="F29" s="48"/>
       <c r="I29" s="49"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="1"/>
       <c r="E30" s="4">
         <v>7</v>
@@ -1290,123 +1299,123 @@
       <c r="F30" s="48"/>
       <c r="I30" s="49"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="1"/>
       <c r="F31" s="48"/>
       <c r="I31" s="49"/>
     </row>
-    <row r="32" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="14.25" customHeight="1">
       <c r="E32" s="4" t="s">
         <v>16</v>
       </c>
       <c r="I32" s="49"/>
     </row>
-    <row r="33" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:12" ht="14.25" customHeight="1">
       <c r="E33" s="4">
         <v>1</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I33" s="49"/>
       <c r="J33" s="21"/>
       <c r="K33" s="21"/>
       <c r="L33" s="21"/>
     </row>
-    <row r="34" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:12" ht="14.25" customHeight="1">
       <c r="E34" s="4">
         <v>2</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="I34" s="49"/>
       <c r="J34" s="21"/>
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
     </row>
-    <row r="35" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:12" ht="14.25" customHeight="1">
       <c r="E35" s="4">
         <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="I35" s="49"/>
       <c r="J35" s="21"/>
       <c r="K35" s="21"/>
       <c r="L35" s="21"/>
     </row>
-    <row r="36" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:12" ht="14.25" customHeight="1">
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:12" ht="10.5" customHeight="1">
       <c r="I37" s="5"/>
     </row>
-    <row r="38" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:12" ht="10.5" customHeight="1">
       <c r="I38" s="5"/>
     </row>
-    <row r="39" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:12" ht="10.5" customHeight="1">
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:12" ht="10.5" customHeight="1">
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:12" ht="10.5" customHeight="1">
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:12">
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:12">
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:12">
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:12">
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:12">
       <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:12">
       <c r="I47" s="5"/>
     </row>
-    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:12">
       <c r="I48" s="5"/>
     </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="9:9">
       <c r="I49" s="5"/>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="9:9">
       <c r="I50" s="5"/>
     </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="9:9">
       <c r="I51" s="5"/>
     </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="9:9">
       <c r="I52" s="5"/>
     </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="9:9">
       <c r="I53" s="5"/>
     </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="9:9">
       <c r="I54" s="5"/>
     </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="9:9">
       <c r="I55" s="5"/>
     </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="9:9">
       <c r="I56" s="5"/>
     </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="9:9">
       <c r="I57" s="5"/>
     </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="9:9">
       <c r="I58" s="5"/>
     </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="9:9">
       <c r="I59" s="5"/>
     </row>
   </sheetData>
@@ -1424,24 +1433,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1497,18 +1506,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1527,17 +1536,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC78C7E-41AD-4518-BFAA-0ABA4B09AB48}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>